<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-study-summary-ig@04f719fc0913dafb5d1cc4fd080ccd561abd3892 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-study-summary-group.xlsx
+++ b/StructureDefinition-study-summary-group.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-11T21:49:34+00:00</t>
+    <t>2022-04-22T15:57:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -484,55 +484,55 @@
     <t>This resource is generally assumed to be active if no value is provided for the active element</t>
   </si>
   <si>
+    <t>./statusCode</t>
+  </si>
+  <si>
+    <t>FiveWs.status</t>
+  </si>
+  <si>
+    <t>Group.type</t>
+  </si>
+  <si>
+    <t>person | animal | practitioner | device | medication | substance</t>
+  </si>
+  <si>
+    <t>Identifies the broad classification of the kind of resources the group includes.</t>
+  </si>
+  <si>
+    <t>Group members SHALL be of the appropriate resource type (Patient for person or animal; or Practitioner, Device, Medication or Substance for the other types.).</t>
+  </si>
+  <si>
+    <t>Identifies what type of resources the group is made up of.</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Types of resources that are part of group.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/group-type|4.0.1</t>
+  </si>
+  <si>
+    <t>person: ./classCode="PSN"  animal: ./classCode="ANM"  device: ./classCode="DEV"  medication: ./classCode="MMAT" and ./playedRole[isNormalRole() and classCode="THER"]  food: ./classCode="FOOD"</t>
+  </si>
+  <si>
+    <t>FiveWs.class</t>
+  </si>
+  <si>
+    <t>Group.actual</t>
+  </si>
+  <si>
+    <t>Descriptive or actual</t>
+  </si>
+  <si>
+    <t>If true, indicates that the resource refers to a specific group of real individuals.  If false, the group defines a set of intended individuals.</t>
+  </si>
+  <si>
+    <t>There are use-cases for groups that define specific collections of individuals, and other groups that define "types" of intended individuals.  The requirements for both kinds of groups are similar, so we use a single resource, distinguished by this flag.</t>
+  </si>
+  <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>./statusCode</t>
-  </si>
-  <si>
-    <t>FiveWs.status</t>
-  </si>
-  <si>
-    <t>Group.type</t>
-  </si>
-  <si>
-    <t>person | animal | practitioner | device | medication | substance</t>
-  </si>
-  <si>
-    <t>Identifies the broad classification of the kind of resources the group includes.</t>
-  </si>
-  <si>
-    <t>Group members SHALL be of the appropriate resource type (Patient for person or animal; or Practitioner, Device, Medication or Substance for the other types.).</t>
-  </si>
-  <si>
-    <t>Identifies what type of resources the group is made up of.</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>Types of resources that are part of group.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/group-type|4.0.1</t>
-  </si>
-  <si>
-    <t>person: ./classCode="PSN"  animal: ./classCode="ANM"  device: ./classCode="DEV"  medication: ./classCode="MMAT" and ./playedRole[isNormalRole() and classCode="THER"]  food: ./classCode="FOOD"</t>
-  </si>
-  <si>
-    <t>FiveWs.class</t>
-  </si>
-  <si>
-    <t>Group.actual</t>
-  </si>
-  <si>
-    <t>Descriptive or actual</t>
-  </si>
-  <si>
-    <t>If true, indicates that the resource refers to a specific group of real individuals.  If false, the group defines a set of intended individuals.</t>
-  </si>
-  <si>
-    <t>There are use-cases for groups that define specific collections of individuals, and other groups that define "types" of intended individuals.  The requirements for both kinds of groups are similar, so we use a single resource, distinguished by this flag.</t>
   </si>
   <si>
     <t xml:space="preserve">grp-1
@@ -2347,7 +2347,7 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s" s="2">
         <v>81</v>
@@ -2384,7 +2384,7 @@
         <v>72</v>
       </c>
       <c r="R12" t="s" s="2">
-        <v>151</v>
+        <v>72</v>
       </c>
       <c r="S12" t="s" s="2">
         <v>72</v>
@@ -2438,15 +2438,15 @@
         <v>93</v>
       </c>
       <c r="AJ12" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AK12" t="s" s="2">
         <v>152</v>
-      </c>
-      <c r="AK12" t="s" s="2">
-        <v>153</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2472,16 +2472,16 @@
         <v>101</v>
       </c>
       <c r="K13" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L13" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="L13" t="s" s="2">
+      <c r="M13" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="M13" t="s" s="2">
+      <c r="N13" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="N13" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="O13" t="s" s="2">
         <v>72</v>
@@ -2506,14 +2506,14 @@
         <v>72</v>
       </c>
       <c r="W13" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="X13" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="X13" t="s" s="2">
+      <c r="Y13" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="Y13" t="s" s="2">
-        <v>161</v>
-      </c>
       <c r="Z13" t="s" s="2">
         <v>72</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>72</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>81</v>
@@ -2545,15 +2545,15 @@
         <v>93</v>
       </c>
       <c r="AJ13" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AK13" t="s" s="2">
         <v>162</v>
-      </c>
-      <c r="AK13" t="s" s="2">
-        <v>163</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2579,14 +2579,14 @@
         <v>146</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="L14" t="s" s="2">
         <v>165</v>
-      </c>
-      <c r="L14" t="s" s="2">
-        <v>166</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" t="s" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O14" t="s" s="2">
         <v>72</v>
@@ -2596,7 +2596,7 @@
         <v>72</v>
       </c>
       <c r="R14" t="s" s="2">
-        <v>72</v>
+        <v>167</v>
       </c>
       <c r="S14" t="s" s="2">
         <v>72</v>
@@ -2635,7 +2635,7 @@
         <v>72</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>81</v>
@@ -2653,7 +2653,7 @@
         <v>169</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15">

</xml_diff>